<commit_message>
workbench ERD 및 테이블 구현
</commit_message>
<xml_diff>
--- a/포트폴리오/데이터베이스 설계/market.xlsx
+++ b/포트폴리오/데이터베이스 설계/market.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="900" uniqueCount="155">
   <si>
     <t>member</t>
   </si>
@@ -86,13 +86,46 @@
     <t>varchar(13)</t>
   </si>
   <si>
+    <t>이메일</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
     <t>회원 주소</t>
   </si>
   <si>
     <t>address</t>
   </si>
   <si>
-    <t>Y</t>
+    <t>회원 적립금</t>
+  </si>
+  <si>
+    <t>point</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>은행명</t>
+  </si>
+  <si>
+    <t>bank</t>
+  </si>
+  <si>
+    <t>varchar(10)</t>
+  </si>
+  <si>
+    <t>계좌번호</t>
+  </si>
+  <si>
+    <t>account</t>
   </si>
   <si>
     <t>회원 등급</t>
@@ -101,40 +134,10 @@
     <t>grade</t>
   </si>
   <si>
-    <t>varchar(10)</t>
-  </si>
-  <si>
     <t>user</t>
   </si>
   <si>
-    <t>회원 적립금</t>
-  </si>
-  <si>
-    <t>point</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>은행명</t>
-  </si>
-  <si>
-    <t>bank</t>
-  </si>
-  <si>
-    <t>varchar(5)</t>
-  </si>
-  <si>
-    <t>계좌번호</t>
-  </si>
-  <si>
-    <t>account</t>
-  </si>
-  <si>
-    <t>회원 상태</t>
+    <t>상태</t>
   </si>
   <si>
     <t>valid</t>
@@ -146,7 +149,7 @@
     <t>I</t>
   </si>
   <si>
-    <t>product</t>
+    <t>item</t>
   </si>
   <si>
     <t>상품 번호</t>
@@ -161,13 +164,13 @@
     <t>판매자 번호</t>
   </si>
   <si>
-    <t>sellerNo</t>
+    <t>seller_no</t>
   </si>
   <si>
     <t>카테고리 번호</t>
   </si>
   <si>
-    <t>categoryNo</t>
+    <t>category_no</t>
   </si>
   <si>
     <t>상품 이름</t>
@@ -200,16 +203,16 @@
     <t>commend</t>
   </si>
   <si>
-    <t>상품 상태</t>
-  </si>
-  <si>
     <t>buy</t>
   </si>
   <si>
     <t>주문번호</t>
   </si>
   <si>
-    <t>productNo</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>item_no</t>
   </si>
   <si>
     <t>주문 수량</t>
@@ -227,24 +230,27 @@
     <t>주문 가격</t>
   </si>
   <si>
+    <t>주문시간</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
     <t>주문 진행 상황</t>
   </si>
   <si>
     <t>state</t>
   </si>
   <si>
-    <t>주문 상태</t>
-  </si>
-  <si>
     <t>wishlist</t>
   </si>
   <si>
     <t>위시리스트 번호</t>
   </si>
   <si>
-    <t>위시리스트 상태</t>
-  </si>
-  <si>
     <t>bag</t>
   </si>
   <si>
@@ -257,28 +263,25 @@
     <t>가격</t>
   </si>
   <si>
-    <t>장바구니 상태</t>
-  </si>
-  <si>
     <t>delivery</t>
   </si>
   <si>
     <t>배송번호</t>
   </si>
   <si>
-    <t>buyNo</t>
+    <t>buy_no</t>
   </si>
   <si>
     <t>배송 출발지</t>
   </si>
   <si>
-    <t>startPlace</t>
+    <t>start</t>
   </si>
   <si>
     <t>배송 도착지</t>
   </si>
   <si>
-    <t>endPlace</t>
+    <t>end</t>
   </si>
   <si>
     <t>택배회사명</t>
@@ -299,10 +302,7 @@
     <t>배송 출발일</t>
   </si>
   <si>
-    <t>start</t>
-  </si>
-  <si>
-    <t>datetime</t>
+    <t>startTime</t>
   </si>
   <si>
     <t>now()</t>
@@ -311,15 +311,12 @@
     <t>배송 종료일</t>
   </si>
   <si>
-    <t>end</t>
+    <t>endTime</t>
   </si>
   <si>
     <t>CURRENT_TIMESTAMP</t>
   </si>
   <si>
-    <t>배송 상태</t>
-  </si>
-  <si>
     <t>category</t>
   </si>
   <si>
@@ -332,6 +329,12 @@
     <t>소분류</t>
   </si>
   <si>
+    <t>detail</t>
+  </si>
+  <si>
+    <t>varchar(15)</t>
+  </si>
+  <si>
     <t>coupon</t>
   </si>
   <si>
@@ -359,9 +362,6 @@
     <t>period</t>
   </si>
   <si>
-    <t>쿠폰 상태</t>
-  </si>
-  <si>
     <t>seller</t>
   </si>
   <si>
@@ -371,16 +371,16 @@
     <t>code</t>
   </si>
   <si>
-    <t>판매자 이름</t>
-  </si>
-  <si>
-    <t>판매자 연락처</t>
-  </si>
-  <si>
-    <t>판매자 계좌번호</t>
-  </si>
-  <si>
-    <t>판매자 주소</t>
+    <t>사업자명</t>
+  </si>
+  <si>
+    <t>사업자 연락처</t>
+  </si>
+  <si>
+    <t>사업자 은행명</t>
+  </si>
+  <si>
+    <t>사업자 계좌번호</t>
   </si>
   <si>
     <t>사업장 주소</t>
@@ -389,9 +389,6 @@
     <t>place</t>
   </si>
   <si>
-    <t>판매자 상태</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -419,22 +416,13 @@
     <t>작성 시간</t>
   </si>
   <si>
-    <t>time</t>
-  </si>
-  <si>
-    <t>게시글 상태</t>
-  </si>
-  <si>
-    <t>coupon_bag</t>
+    <t>couponBag</t>
   </si>
   <si>
     <t>쿠폰함 번호</t>
   </si>
   <si>
-    <t>couponNo</t>
-  </si>
-  <si>
-    <t>쿠폰함 상태</t>
+    <t>coupon_no</t>
   </si>
   <si>
     <t>comment</t>
@@ -443,7 +431,7 @@
     <t>댓글 번호</t>
   </si>
   <si>
-    <t>boardNo</t>
+    <t>board_no</t>
   </si>
   <si>
     <t>댓글 대상자</t>
@@ -461,9 +449,6 @@
     <t>댓글 등록 시간</t>
   </si>
   <si>
-    <t>댓글 상태</t>
-  </si>
-  <si>
     <t>file</t>
   </si>
   <si>
@@ -474,6 +459,21 @@
   </si>
   <si>
     <t>route</t>
+  </si>
+  <si>
+    <t>option</t>
+  </si>
+  <si>
+    <t>번호</t>
+  </si>
+  <si>
+    <t>선택 상품</t>
+  </si>
+  <si>
+    <t>select</t>
+  </si>
+  <si>
+    <t>세부 옵션</t>
   </si>
 </sst>
 </file>
@@ -842,7 +842,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H125"/>
+  <dimension ref="A1:H137"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -999,7 +999,7 @@
         <v>27</v>
       </c>
       <c r="G7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
@@ -1019,13 +1019,13 @@
         <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G8" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="H8" t="s">
         <v>12</v>
@@ -1036,22 +1036,22 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
         <v>32</v>
       </c>
-      <c r="C9" t="s">
+      <c r="F9" t="s">
+        <v>14</v>
+      </c>
+      <c r="G9" t="s">
         <v>33</v>
-      </c>
-      <c r="D9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" t="s">
-        <v>35</v>
       </c>
       <c r="H9" t="s">
         <v>12</v>
@@ -1062,16 +1062,16 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
         <v>36</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -1088,10 +1088,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" t="s">
         <v>12</v>
@@ -1114,22 +1114,22 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" t="s">
         <v>41</v>
-      </c>
-      <c r="C12" t="s">
-        <v>42</v>
-      </c>
-      <c r="D12" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" t="s">
-        <v>14</v>
-      </c>
-      <c r="G12" t="s">
-        <v>44</v>
       </c>
       <c r="H12" t="s">
         <v>12</v>
@@ -1139,79 +1139,79 @@
       <c r="A13" t="s">
         <v>12</v>
       </c>
+      <c r="B13" t="s">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>44</v>
+      </c>
+      <c r="F13" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" t="s">
-        <v>4</v>
-      </c>
-      <c r="E15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" t="s">
-        <v>6</v>
-      </c>
-      <c r="G15" t="s">
-        <v>7</v>
-      </c>
-      <c r="H15" t="s">
-        <v>8</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E16" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="F16" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
         <v>48</v>
       </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>50</v>
-      </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F17" t="s">
         <v>14</v>
@@ -1225,19 +1225,19 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B18" t="s">
+        <v>50</v>
+      </c>
+      <c r="C18" t="s">
         <v>51</v>
       </c>
-      <c r="C18" t="s">
-        <v>52</v>
-      </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F18" t="s">
         <v>14</v>
@@ -1251,25 +1251,25 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19" t="s">
         <v>53</v>
       </c>
-      <c r="C19" t="s">
-        <v>20</v>
-      </c>
       <c r="D19" t="s">
         <v>12</v>
       </c>
       <c r="E19" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H19" t="s">
         <v>12</v>
@@ -1283,19 +1283,19 @@
         <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="F20" t="s">
         <v>14</v>
       </c>
       <c r="G20" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H20" t="s">
         <v>12</v>
@@ -1306,22 +1306,22 @@
         <v>12</v>
       </c>
       <c r="B21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
         <v>56</v>
       </c>
-      <c r="C21" t="s">
-        <v>57</v>
-      </c>
       <c r="D21" t="s">
         <v>12</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="F21" t="s">
         <v>14</v>
       </c>
       <c r="G21" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="H21" t="s">
         <v>12</v>
@@ -1332,22 +1332,22 @@
         <v>12</v>
       </c>
       <c r="B22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" t="s">
         <v>59</v>
       </c>
-      <c r="C22" t="s">
-        <v>60</v>
-      </c>
-      <c r="D22" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" t="s">
-        <v>34</v>
-      </c>
       <c r="F22" t="s">
         <v>14</v>
       </c>
       <c r="G22" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H22" t="s">
         <v>12</v>
@@ -1358,22 +1358,22 @@
         <v>12</v>
       </c>
       <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
         <v>61</v>
       </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
       <c r="D23" t="s">
         <v>12</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F23" t="s">
         <v>14</v>
       </c>
       <c r="G23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H23" t="s">
         <v>12</v>
@@ -1384,22 +1384,22 @@
         <v>12</v>
       </c>
       <c r="B24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C24" t="s">
         <v>63</v>
       </c>
-      <c r="C24" t="s">
-        <v>42</v>
-      </c>
       <c r="D24" t="s">
         <v>12</v>
       </c>
       <c r="E24" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
       </c>
       <c r="G24" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H24" t="s">
         <v>12</v>
@@ -1409,85 +1409,85 @@
       <c r="A25" t="s">
         <v>12</v>
       </c>
+      <c r="B25" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G25" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" t="s">
-        <v>4</v>
-      </c>
-      <c r="E27" t="s">
-        <v>5</v>
-      </c>
-      <c r="F27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G27" t="s">
-        <v>7</v>
-      </c>
-      <c r="H27" t="s">
-        <v>8</v>
+        <v>64</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B28" t="s">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>3</v>
       </c>
       <c r="D28" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="F28" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G28" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H28" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" t="s">
         <v>48</v>
       </c>
-      <c r="B29" t="s">
-        <v>10</v>
-      </c>
-      <c r="C29" t="s">
-        <v>11</v>
-      </c>
       <c r="D29" t="s">
         <v>12</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F29" t="s">
         <v>14</v>
       </c>
       <c r="G29" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H29" t="s">
         <v>12</v>
@@ -1495,10 +1495,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="C30" t="s">
         <v>66</v>
@@ -1507,13 +1507,13 @@
         <v>12</v>
       </c>
       <c r="E30" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="F30" t="s">
         <v>14</v>
       </c>
       <c r="G30" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="H30" t="s">
         <v>12</v>
@@ -1521,25 +1521,25 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
         <v>67</v>
       </c>
-      <c r="C31" t="s">
-        <v>68</v>
-      </c>
       <c r="D31" t="s">
         <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F31" t="s">
         <v>14</v>
       </c>
       <c r="G31" t="s">
-        <v>69</v>
+        <v>12</v>
       </c>
       <c r="H31" t="s">
         <v>12</v>
@@ -1550,22 +1550,22 @@
         <v>12</v>
       </c>
       <c r="B32" t="s">
+        <v>68</v>
+      </c>
+      <c r="C32" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>32</v>
+      </c>
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32" t="s">
         <v>70</v>
-      </c>
-      <c r="C32" t="s">
-        <v>57</v>
-      </c>
-      <c r="D32" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" t="s">
-        <v>14</v>
-      </c>
-      <c r="G32" t="s">
-        <v>15</v>
       </c>
       <c r="H32" t="s">
         <v>12</v>
@@ -1579,19 +1579,19 @@
         <v>71</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="F33" t="s">
         <v>14</v>
       </c>
       <c r="G33" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H33" t="s">
         <v>12</v>
@@ -1605,19 +1605,19 @@
         <v>72</v>
       </c>
       <c r="C34" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F34" t="s">
         <v>14</v>
       </c>
       <c r="G34" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="H34" t="s">
         <v>12</v>
@@ -1628,22 +1628,22 @@
         <v>12</v>
       </c>
       <c r="B35" t="s">
+        <v>73</v>
+      </c>
+      <c r="C35" t="s">
         <v>74</v>
       </c>
-      <c r="C35" t="s">
-        <v>42</v>
-      </c>
       <c r="D35" t="s">
         <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="F35" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G35" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="H35" t="s">
         <v>12</v>
@@ -1653,105 +1653,105 @@
       <c r="A36" t="s">
         <v>12</v>
       </c>
+      <c r="B36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" t="s">
+        <v>12</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+      <c r="F36" t="s">
+        <v>14</v>
+      </c>
+      <c r="G36" t="s">
+        <v>15</v>
+      </c>
+      <c r="H36" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>12</v>
+      </c>
+      <c r="B37" t="s">
+        <v>42</v>
+      </c>
+      <c r="C37" t="s">
+        <v>43</v>
+      </c>
+      <c r="D37" t="s">
+        <v>12</v>
+      </c>
+      <c r="E37" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" t="s">
+        <v>14</v>
+      </c>
+      <c r="G37" t="s">
+        <v>45</v>
+      </c>
+      <c r="H37" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
-        <v>2</v>
-      </c>
-      <c r="C38" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" t="s">
-        <v>4</v>
-      </c>
-      <c r="E38" t="s">
-        <v>5</v>
-      </c>
-      <c r="F38" t="s">
-        <v>6</v>
-      </c>
-      <c r="G38" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>9</v>
-      </c>
-      <c r="B39" t="s">
-        <v>76</v>
-      </c>
-      <c r="C39" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" t="s">
-        <v>12</v>
-      </c>
-      <c r="E39" t="s">
-        <v>34</v>
-      </c>
-      <c r="F39" t="s">
-        <v>14</v>
-      </c>
-      <c r="G39" t="s">
-        <v>12</v>
-      </c>
-      <c r="H39" t="s">
-        <v>12</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B40" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D40" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E40" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F40" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G40" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H40" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
+        <v>9</v>
+      </c>
+      <c r="B41" t="s">
+        <v>79</v>
+      </c>
+      <c r="C41" t="s">
         <v>48</v>
       </c>
-      <c r="B41" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" t="s">
-        <v>66</v>
-      </c>
       <c r="D41" t="s">
         <v>12</v>
       </c>
       <c r="E41" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F41" t="s">
         <v>14</v>
@@ -1765,25 +1765,25 @@
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B42" t="s">
-        <v>77</v>
+        <v>10</v>
       </c>
       <c r="C42" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
       </c>
       <c r="E42" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F42" t="s">
         <v>14</v>
       </c>
       <c r="G42" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="H42" t="s">
         <v>12</v>
@@ -1791,107 +1791,107 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" t="s">
+        <v>67</v>
+      </c>
+      <c r="D43" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" t="s">
+        <v>32</v>
+      </c>
+      <c r="F43" t="s">
+        <v>14</v>
+      </c>
+      <c r="G43" t="s">
+        <v>12</v>
+      </c>
+      <c r="H43" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>12</v>
+      </c>
+      <c r="B44" t="s">
+        <v>42</v>
+      </c>
+      <c r="C44" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" t="s">
+        <v>44</v>
+      </c>
+      <c r="F44" t="s">
+        <v>14</v>
+      </c>
+      <c r="G44" t="s">
+        <v>45</v>
+      </c>
+      <c r="H44" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>1</v>
-      </c>
-      <c r="B45" t="s">
-        <v>2</v>
-      </c>
-      <c r="C45" t="s">
-        <v>3</v>
-      </c>
-      <c r="D45" t="s">
-        <v>4</v>
-      </c>
-      <c r="E45" t="s">
-        <v>5</v>
-      </c>
-      <c r="F45" t="s">
-        <v>6</v>
-      </c>
-      <c r="G45" t="s">
-        <v>7</v>
-      </c>
-      <c r="H45" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>9</v>
-      </c>
-      <c r="B46" t="s">
-        <v>79</v>
-      </c>
-      <c r="C46" t="s">
-        <v>47</v>
-      </c>
-      <c r="D46" t="s">
-        <v>12</v>
-      </c>
-      <c r="E46" t="s">
-        <v>34</v>
-      </c>
-      <c r="F46" t="s">
-        <v>14</v>
-      </c>
-      <c r="G46" t="s">
-        <v>12</v>
-      </c>
-      <c r="H46" t="s">
-        <v>12</v>
+        <v>80</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="D47" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E47" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F47" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G47" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H47" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
+        <v>9</v>
+      </c>
+      <c r="B48" t="s">
+        <v>81</v>
+      </c>
+      <c r="C48" t="s">
         <v>48</v>
       </c>
-      <c r="B48" t="s">
-        <v>46</v>
-      </c>
-      <c r="C48" t="s">
-        <v>66</v>
-      </c>
       <c r="D48" t="s">
         <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F48" t="s">
         <v>14</v>
@@ -1905,25 +1905,25 @@
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C49" t="s">
-        <v>68</v>
+        <v>11</v>
       </c>
       <c r="D49" t="s">
         <v>12</v>
       </c>
       <c r="E49" t="s">
-        <v>34</v>
+        <v>13</v>
       </c>
       <c r="F49" t="s">
         <v>14</v>
       </c>
       <c r="G49" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="H49" t="s">
         <v>12</v>
@@ -1931,25 +1931,25 @@
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>81</v>
+        <v>47</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F50" t="s">
         <v>14</v>
       </c>
       <c r="G50" t="s">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="H50" t="s">
         <v>12</v>
@@ -1963,19 +1963,19 @@
         <v>82</v>
       </c>
       <c r="C51" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
       </c>
       <c r="E51" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F51" t="s">
         <v>14</v>
       </c>
       <c r="G51" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="H51" t="s">
         <v>12</v>
@@ -1985,111 +1985,111 @@
       <c r="A52" t="s">
         <v>12</v>
       </c>
+      <c r="B52" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" t="s">
+        <v>56</v>
+      </c>
+      <c r="D52" t="s">
+        <v>12</v>
+      </c>
+      <c r="E52" t="s">
+        <v>32</v>
+      </c>
+      <c r="F52" t="s">
+        <v>14</v>
+      </c>
+      <c r="G52" t="s">
+        <v>33</v>
+      </c>
+      <c r="H52" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>83</v>
+        <v>12</v>
+      </c>
+      <c r="B53" t="s">
+        <v>42</v>
+      </c>
+      <c r="C53" t="s">
+        <v>43</v>
+      </c>
+      <c r="D53" t="s">
+        <v>12</v>
+      </c>
+      <c r="E53" t="s">
+        <v>44</v>
+      </c>
+      <c r="F53" t="s">
+        <v>14</v>
+      </c>
+      <c r="G53" t="s">
+        <v>45</v>
+      </c>
+      <c r="H53" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>1</v>
-      </c>
-      <c r="B54" t="s">
-        <v>2</v>
-      </c>
-      <c r="C54" t="s">
-        <v>3</v>
-      </c>
-      <c r="D54" t="s">
-        <v>4</v>
-      </c>
-      <c r="E54" t="s">
-        <v>5</v>
-      </c>
-      <c r="F54" t="s">
-        <v>6</v>
-      </c>
-      <c r="G54" t="s">
-        <v>7</v>
-      </c>
-      <c r="H54" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>9</v>
-      </c>
-      <c r="B55" t="s">
         <v>84</v>
-      </c>
-      <c r="C55" t="s">
-        <v>47</v>
-      </c>
-      <c r="D55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" t="s">
-        <v>34</v>
-      </c>
-      <c r="F55" t="s">
-        <v>14</v>
-      </c>
-      <c r="G55" t="s">
-        <v>12</v>
-      </c>
-      <c r="H55" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>85</v>
+        <v>3</v>
       </c>
       <c r="D56" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E56" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="F56" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G56" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H56" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C57" t="s">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
       </c>
       <c r="E57" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F57" t="s">
         <v>14</v>
       </c>
       <c r="G57" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H57" t="s">
         <v>12</v>
@@ -2097,25 +2097,25 @@
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>65</v>
       </c>
       <c r="C58" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D58" t="s">
         <v>12</v>
       </c>
       <c r="E58" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F58" t="s">
         <v>14</v>
       </c>
       <c r="G58" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H58" t="s">
         <v>12</v>
@@ -2126,10 +2126,10 @@
         <v>12</v>
       </c>
       <c r="B59" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C59" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D59" t="s">
         <v>12</v>
@@ -2152,10 +2152,10 @@
         <v>12</v>
       </c>
       <c r="B60" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C60" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D60" t="s">
         <v>12</v>
@@ -2178,16 +2178,16 @@
         <v>12</v>
       </c>
       <c r="B61" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="C61" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="D61" t="s">
         <v>12</v>
       </c>
       <c r="E61" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F61" t="s">
         <v>14</v>
@@ -2204,22 +2204,22 @@
         <v>12</v>
       </c>
       <c r="B62" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C62" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D62" t="s">
         <v>12</v>
       </c>
       <c r="E62" t="s">
-        <v>97</v>
+        <v>21</v>
       </c>
       <c r="F62" t="s">
         <v>14</v>
       </c>
       <c r="G62" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="H62" t="s">
         <v>12</v>
@@ -2230,22 +2230,22 @@
         <v>12</v>
       </c>
       <c r="B63" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C63" t="s">
-        <v>100</v>
+        <v>23</v>
       </c>
       <c r="D63" t="s">
         <v>12</v>
       </c>
       <c r="E63" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="F63" t="s">
         <v>14</v>
       </c>
       <c r="G63" t="s">
-        <v>101</v>
+        <v>15</v>
       </c>
       <c r="H63" t="s">
         <v>12</v>
@@ -2256,22 +2256,22 @@
         <v>12</v>
       </c>
       <c r="B64" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C64" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="D64" t="s">
         <v>12</v>
       </c>
       <c r="E64" t="s">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="F64" t="s">
         <v>14</v>
       </c>
       <c r="G64" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="H64" t="s">
         <v>12</v>
@@ -2281,111 +2281,111 @@
       <c r="A65" t="s">
         <v>12</v>
       </c>
+      <c r="B65" t="s">
+        <v>99</v>
+      </c>
+      <c r="C65" t="s">
+        <v>100</v>
+      </c>
+      <c r="D65" t="s">
+        <v>12</v>
+      </c>
+      <c r="E65" t="s">
+        <v>75</v>
+      </c>
+      <c r="F65" t="s">
+        <v>14</v>
+      </c>
+      <c r="G65" t="s">
+        <v>101</v>
+      </c>
+      <c r="H65" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>103</v>
+        <v>12</v>
+      </c>
+      <c r="B66" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" t="s">
+        <v>43</v>
+      </c>
+      <c r="D66" t="s">
+        <v>12</v>
+      </c>
+      <c r="E66" t="s">
+        <v>44</v>
+      </c>
+      <c r="F66" t="s">
+        <v>14</v>
+      </c>
+      <c r="G66" t="s">
+        <v>45</v>
+      </c>
+      <c r="H66" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>1</v>
-      </c>
-      <c r="B67" t="s">
-        <v>2</v>
-      </c>
-      <c r="C67" t="s">
-        <v>3</v>
-      </c>
-      <c r="D67" t="s">
-        <v>4</v>
-      </c>
-      <c r="E67" t="s">
-        <v>5</v>
-      </c>
-      <c r="F67" t="s">
-        <v>6</v>
-      </c>
-      <c r="G67" t="s">
-        <v>7</v>
-      </c>
-      <c r="H67" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>9</v>
-      </c>
-      <c r="B68" t="s">
-        <v>51</v>
-      </c>
-      <c r="C68" t="s">
-        <v>47</v>
-      </c>
-      <c r="D68" t="s">
-        <v>12</v>
-      </c>
-      <c r="E68" t="s">
-        <v>34</v>
-      </c>
-      <c r="F68" t="s">
-        <v>14</v>
-      </c>
-      <c r="G68" t="s">
-        <v>12</v>
-      </c>
-      <c r="H68" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>104</v>
+        <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>105</v>
+        <v>3</v>
       </c>
       <c r="D69" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E69" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F69" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G69" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H69" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B70" t="s">
-        <v>106</v>
+        <v>52</v>
       </c>
       <c r="C70" t="s">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="D70" t="s">
         <v>12</v>
       </c>
       <c r="E70" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F70" t="s">
         <v>14</v>
       </c>
       <c r="G70" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H70" t="s">
         <v>12</v>
@@ -2395,137 +2395,137 @@
       <c r="A71" t="s">
         <v>12</v>
       </c>
+      <c r="B71" t="s">
+        <v>103</v>
+      </c>
+      <c r="C71" t="s">
+        <v>104</v>
+      </c>
+      <c r="D71" t="s">
+        <v>12</v>
+      </c>
+      <c r="E71" t="s">
+        <v>36</v>
+      </c>
+      <c r="F71" t="s">
+        <v>14</v>
+      </c>
+      <c r="G71" t="s">
+        <v>15</v>
+      </c>
+      <c r="H71" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
+        <v>12</v>
+      </c>
+      <c r="B72" t="s">
+        <v>105</v>
+      </c>
+      <c r="C72" t="s">
+        <v>106</v>
+      </c>
+      <c r="D72" t="s">
+        <v>12</v>
+      </c>
+      <c r="E72" t="s">
         <v>107</v>
+      </c>
+      <c r="F72" t="s">
+        <v>14</v>
+      </c>
+      <c r="G72" t="s">
+        <v>15</v>
+      </c>
+      <c r="H72" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B73" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C73" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="D73" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E73" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F73" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="G73" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H73" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>9</v>
-      </c>
-      <c r="B74" t="s">
-        <v>108</v>
-      </c>
-      <c r="C74" t="s">
-        <v>47</v>
-      </c>
-      <c r="D74" t="s">
-        <v>12</v>
-      </c>
-      <c r="E74" t="s">
-        <v>34</v>
-      </c>
-      <c r="F74" t="s">
-        <v>14</v>
-      </c>
-      <c r="G74" t="s">
-        <v>12</v>
-      </c>
-      <c r="H74" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>12</v>
-      </c>
-      <c r="B75" t="s">
-        <v>109</v>
-      </c>
-      <c r="C75" t="s">
-        <v>110</v>
-      </c>
-      <c r="D75" t="s">
-        <v>12</v>
-      </c>
-      <c r="E75" t="s">
-        <v>21</v>
-      </c>
-      <c r="F75" t="s">
-        <v>14</v>
-      </c>
-      <c r="G75" t="s">
-        <v>15</v>
-      </c>
-      <c r="H75" t="s">
-        <v>12</v>
+        <v>108</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B76" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="C76" t="s">
-        <v>112</v>
+        <v>3</v>
       </c>
       <c r="D76" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E76" t="s">
-        <v>113</v>
+        <v>5</v>
       </c>
       <c r="F76" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G76" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="H76" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="C77" t="s">
-        <v>115</v>
+        <v>48</v>
       </c>
       <c r="D77" t="s">
         <v>12</v>
       </c>
       <c r="E77" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F77" t="s">
         <v>14</v>
       </c>
       <c r="G77" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H77" t="s">
         <v>12</v>
@@ -2536,22 +2536,22 @@
         <v>12</v>
       </c>
       <c r="B78" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C78" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="D78" t="s">
         <v>12</v>
       </c>
       <c r="E78" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F78" t="s">
         <v>14</v>
       </c>
       <c r="G78" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="H78" t="s">
         <v>12</v>
@@ -2561,137 +2561,137 @@
       <c r="A79" t="s">
         <v>12</v>
       </c>
+      <c r="B79" t="s">
+        <v>112</v>
+      </c>
+      <c r="C79" t="s">
+        <v>113</v>
+      </c>
+      <c r="D79" t="s">
+        <v>12</v>
+      </c>
+      <c r="E79" t="s">
+        <v>114</v>
+      </c>
+      <c r="F79" t="s">
+        <v>14</v>
+      </c>
+      <c r="G79" t="s">
+        <v>33</v>
+      </c>
+      <c r="H79" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>117</v>
+        <v>12</v>
+      </c>
+      <c r="B80" t="s">
+        <v>115</v>
+      </c>
+      <c r="C80" t="s">
+        <v>116</v>
+      </c>
+      <c r="D80" t="s">
+        <v>12</v>
+      </c>
+      <c r="E80" t="s">
+        <v>21</v>
+      </c>
+      <c r="F80" t="s">
+        <v>14</v>
+      </c>
+      <c r="G80" t="s">
+        <v>15</v>
+      </c>
+      <c r="H80" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B81" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C81" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="D81" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E81" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F81" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G81" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="H81" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>9</v>
-      </c>
-      <c r="B82" t="s">
-        <v>49</v>
-      </c>
-      <c r="C82" t="s">
-        <v>47</v>
-      </c>
-      <c r="D82" t="s">
-        <v>12</v>
-      </c>
-      <c r="E82" t="s">
-        <v>34</v>
-      </c>
-      <c r="F82" t="s">
-        <v>14</v>
-      </c>
-      <c r="G82" t="s">
-        <v>12</v>
-      </c>
-      <c r="H82" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>48</v>
-      </c>
-      <c r="B83" t="s">
-        <v>10</v>
-      </c>
-      <c r="C83" t="s">
-        <v>11</v>
-      </c>
-      <c r="D83" t="s">
-        <v>12</v>
-      </c>
-      <c r="E83" t="s">
-        <v>13</v>
-      </c>
-      <c r="F83" t="s">
-        <v>14</v>
-      </c>
-      <c r="G83" t="s">
-        <v>15</v>
-      </c>
-      <c r="H83" t="s">
-        <v>12</v>
+        <v>117</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B84" t="s">
-        <v>118</v>
+        <v>2</v>
       </c>
       <c r="C84" t="s">
-        <v>119</v>
+        <v>3</v>
       </c>
       <c r="D84" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E84" t="s">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="F84" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G84" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H84" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B85" t="s">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="C85" t="s">
-        <v>20</v>
+        <v>48</v>
       </c>
       <c r="D85" t="s">
         <v>12</v>
       </c>
       <c r="E85" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F85" t="s">
         <v>14</v>
       </c>
       <c r="G85" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H85" t="s">
         <v>12</v>
@@ -2699,19 +2699,19 @@
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B86" t="s">
-        <v>121</v>
+        <v>10</v>
       </c>
       <c r="C86" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="D86" t="s">
         <v>12</v>
       </c>
       <c r="E86" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="F86" t="s">
         <v>14</v>
@@ -2728,10 +2728,10 @@
         <v>12</v>
       </c>
       <c r="B87" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C87" t="s">
-        <v>40</v>
+        <v>119</v>
       </c>
       <c r="D87" t="s">
         <v>12</v>
@@ -2754,10 +2754,10 @@
         <v>12</v>
       </c>
       <c r="B88" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C88" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D88" t="s">
         <v>12</v>
@@ -2780,16 +2780,16 @@
         <v>12</v>
       </c>
       <c r="B89" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C89" t="s">
-        <v>125</v>
+        <v>23</v>
       </c>
       <c r="D89" t="s">
         <v>12</v>
       </c>
       <c r="E89" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="F89" t="s">
         <v>14</v>
@@ -2806,22 +2806,22 @@
         <v>12</v>
       </c>
       <c r="B90" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C90" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="D90" t="s">
         <v>12</v>
       </c>
       <c r="E90" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F90" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="G90" t="s">
-        <v>127</v>
+        <v>12</v>
       </c>
       <c r="H90" t="s">
         <v>12</v>
@@ -2831,131 +2831,131 @@
       <c r="A91" t="s">
         <v>12</v>
       </c>
+      <c r="B91" t="s">
+        <v>123</v>
+      </c>
+      <c r="C91" t="s">
+        <v>38</v>
+      </c>
+      <c r="D91" t="s">
+        <v>12</v>
+      </c>
+      <c r="E91" t="s">
+        <v>21</v>
+      </c>
+      <c r="F91" t="s">
+        <v>14</v>
+      </c>
+      <c r="G91" t="s">
+        <v>15</v>
+      </c>
+      <c r="H91" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>128</v>
+        <v>12</v>
+      </c>
+      <c r="B92" t="s">
+        <v>124</v>
+      </c>
+      <c r="C92" t="s">
+        <v>125</v>
+      </c>
+      <c r="D92" t="s">
+        <v>12</v>
+      </c>
+      <c r="E92" t="s">
+        <v>21</v>
+      </c>
+      <c r="F92" t="s">
+        <v>14</v>
+      </c>
+      <c r="G92" t="s">
+        <v>15</v>
+      </c>
+      <c r="H92" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B93" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C93" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="D93" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E93" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F93" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G93" t="s">
-        <v>7</v>
+        <v>126</v>
       </c>
       <c r="H93" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>9</v>
-      </c>
-      <c r="B94" t="s">
-        <v>129</v>
-      </c>
-      <c r="C94" t="s">
-        <v>47</v>
-      </c>
-      <c r="D94" t="s">
-        <v>12</v>
-      </c>
-      <c r="E94" t="s">
-        <v>34</v>
-      </c>
-      <c r="F94" t="s">
-        <v>14</v>
-      </c>
-      <c r="G94" t="s">
-        <v>12</v>
-      </c>
-      <c r="H94" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>48</v>
-      </c>
-      <c r="B95" t="s">
-        <v>51</v>
-      </c>
-      <c r="C95" t="s">
-        <v>52</v>
-      </c>
-      <c r="D95" t="s">
-        <v>12</v>
-      </c>
-      <c r="E95" t="s">
-        <v>34</v>
-      </c>
-      <c r="F95" t="s">
-        <v>14</v>
-      </c>
-      <c r="G95" t="s">
-        <v>12</v>
-      </c>
-      <c r="H95" t="s">
-        <v>12</v>
+        <v>127</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B96" t="s">
-        <v>46</v>
+        <v>2</v>
       </c>
       <c r="C96" t="s">
-        <v>66</v>
+        <v>3</v>
       </c>
       <c r="D96" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E96" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="F96" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G96" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H96" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
+        <v>9</v>
+      </c>
+      <c r="B97" t="s">
+        <v>128</v>
+      </c>
+      <c r="C97" t="s">
         <v>48</v>
       </c>
-      <c r="B97" t="s">
-        <v>130</v>
-      </c>
-      <c r="C97" t="s">
-        <v>131</v>
-      </c>
       <c r="D97" t="s">
         <v>12</v>
       </c>
       <c r="E97" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F97" t="s">
         <v>14</v>
@@ -2969,25 +2969,25 @@
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B98" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="C98" t="s">
-        <v>110</v>
+        <v>53</v>
       </c>
       <c r="D98" t="s">
         <v>12</v>
       </c>
       <c r="E98" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="F98" t="s">
         <v>14</v>
       </c>
       <c r="G98" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H98" t="s">
         <v>12</v>
@@ -2995,25 +2995,25 @@
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B99" t="s">
-        <v>133</v>
+        <v>47</v>
       </c>
       <c r="C99" t="s">
-        <v>134</v>
+        <v>67</v>
       </c>
       <c r="D99" t="s">
         <v>12</v>
       </c>
       <c r="E99" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="F99" t="s">
         <v>14</v>
       </c>
       <c r="G99" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H99" t="s">
         <v>12</v>
@@ -3021,25 +3021,25 @@
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B100" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="C100" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="D100" t="s">
         <v>12</v>
       </c>
       <c r="E100" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="F100" t="s">
         <v>14</v>
       </c>
       <c r="G100" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="H100" t="s">
         <v>12</v>
@@ -3050,22 +3050,22 @@
         <v>12</v>
       </c>
       <c r="B101" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C101" t="s">
-        <v>42</v>
+        <v>111</v>
       </c>
       <c r="D101" t="s">
         <v>12</v>
       </c>
       <c r="E101" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="F101" t="s">
         <v>14</v>
       </c>
       <c r="G101" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="H101" t="s">
         <v>12</v>
@@ -3075,137 +3075,137 @@
       <c r="A102" t="s">
         <v>12</v>
       </c>
+      <c r="B102" t="s">
+        <v>132</v>
+      </c>
+      <c r="C102" t="s">
+        <v>133</v>
+      </c>
+      <c r="D102" t="s">
+        <v>12</v>
+      </c>
+      <c r="E102" t="s">
+        <v>59</v>
+      </c>
+      <c r="F102" t="s">
+        <v>14</v>
+      </c>
+      <c r="G102" t="s">
+        <v>15</v>
+      </c>
+      <c r="H102" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>138</v>
+        <v>12</v>
+      </c>
+      <c r="B103" t="s">
+        <v>134</v>
+      </c>
+      <c r="C103" t="s">
+        <v>74</v>
+      </c>
+      <c r="D103" t="s">
+        <v>12</v>
+      </c>
+      <c r="E103" t="s">
+        <v>75</v>
+      </c>
+      <c r="F103" t="s">
+        <v>14</v>
+      </c>
+      <c r="G103" t="s">
+        <v>98</v>
+      </c>
+      <c r="H103" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B104" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C104" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="D104" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E104" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F104" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G104" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="H104" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>9</v>
-      </c>
-      <c r="B105" t="s">
-        <v>139</v>
-      </c>
-      <c r="C105" t="s">
-        <v>47</v>
-      </c>
-      <c r="D105" t="s">
-        <v>12</v>
-      </c>
-      <c r="E105" t="s">
-        <v>34</v>
-      </c>
-      <c r="F105" t="s">
-        <v>14</v>
-      </c>
-      <c r="G105" t="s">
-        <v>12</v>
-      </c>
-      <c r="H105" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="s">
-        <v>48</v>
-      </c>
-      <c r="B106" t="s">
-        <v>10</v>
-      </c>
-      <c r="C106" t="s">
-        <v>11</v>
-      </c>
-      <c r="D106" t="s">
-        <v>12</v>
-      </c>
-      <c r="E106" t="s">
-        <v>13</v>
-      </c>
-      <c r="F106" t="s">
-        <v>14</v>
-      </c>
-      <c r="G106" t="s">
-        <v>15</v>
-      </c>
-      <c r="H106" t="s">
-        <v>12</v>
+        <v>135</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B107" t="s">
-        <v>108</v>
+        <v>2</v>
       </c>
       <c r="C107" t="s">
-        <v>140</v>
+        <v>3</v>
       </c>
       <c r="D107" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E107" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="F107" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G107" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H107" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B108" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C108" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D108" t="s">
         <v>12</v>
       </c>
       <c r="E108" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="F108" t="s">
         <v>14</v>
       </c>
       <c r="G108" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="H108" t="s">
         <v>12</v>
@@ -3213,139 +3213,139 @@
     </row>
     <row r="109">
       <c r="A109" t="s">
+        <v>49</v>
+      </c>
+      <c r="B109" t="s">
+        <v>10</v>
+      </c>
+      <c r="C109" t="s">
+        <v>11</v>
+      </c>
+      <c r="D109" t="s">
+        <v>12</v>
+      </c>
+      <c r="E109" t="s">
+        <v>13</v>
+      </c>
+      <c r="F109" t="s">
+        <v>14</v>
+      </c>
+      <c r="G109" t="s">
+        <v>15</v>
+      </c>
+      <c r="H109" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="s">
-        <v>142</v>
+        <v>49</v>
+      </c>
+      <c r="B110" t="s">
+        <v>109</v>
+      </c>
+      <c r="C110" t="s">
+        <v>137</v>
+      </c>
+      <c r="D110" t="s">
+        <v>12</v>
+      </c>
+      <c r="E110" t="s">
+        <v>32</v>
+      </c>
+      <c r="F110" t="s">
+        <v>14</v>
+      </c>
+      <c r="G110" t="s">
+        <v>12</v>
+      </c>
+      <c r="H110" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B111" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C111" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="D111" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E111" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F111" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G111" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="H111" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="s">
-        <v>9</v>
-      </c>
-      <c r="B112" t="s">
-        <v>143</v>
-      </c>
-      <c r="C112" t="s">
-        <v>47</v>
-      </c>
-      <c r="D112" t="s">
-        <v>12</v>
-      </c>
-      <c r="E112" t="s">
-        <v>34</v>
-      </c>
-      <c r="F112" t="s">
-        <v>14</v>
-      </c>
-      <c r="G112" t="s">
-        <v>12</v>
-      </c>
-      <c r="H112" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="s">
-        <v>48</v>
-      </c>
-      <c r="B113" t="s">
-        <v>129</v>
-      </c>
-      <c r="C113" t="s">
-        <v>144</v>
-      </c>
-      <c r="D113" t="s">
-        <v>12</v>
-      </c>
-      <c r="E113" t="s">
-        <v>34</v>
-      </c>
-      <c r="F113" t="s">
-        <v>14</v>
-      </c>
-      <c r="G113" t="s">
-        <v>12</v>
-      </c>
-      <c r="H113" t="s">
-        <v>12</v>
+        <v>138</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
       <c r="B114" t="s">
-        <v>145</v>
+        <v>2</v>
       </c>
       <c r="C114" t="s">
-        <v>146</v>
+        <v>3</v>
       </c>
       <c r="D114" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E114" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F114" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G114" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H114" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B115" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C115" t="s">
-        <v>131</v>
+        <v>48</v>
       </c>
       <c r="D115" t="s">
         <v>12</v>
       </c>
       <c r="E115" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="F115" t="s">
         <v>14</v>
       </c>
       <c r="G115" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H115" t="s">
         <v>12</v>
@@ -3353,25 +3353,25 @@
     </row>
     <row r="116">
       <c r="A116" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B116" t="s">
-        <v>148</v>
+        <v>128</v>
       </c>
       <c r="C116" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="D116" t="s">
         <v>12</v>
       </c>
       <c r="E116" t="s">
-        <v>58</v>
+        <v>32</v>
       </c>
       <c r="F116" t="s">
         <v>14</v>
       </c>
       <c r="G116" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H116" t="s">
         <v>12</v>
@@ -3379,25 +3379,25 @@
     </row>
     <row r="117">
       <c r="A117" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="B117" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C117" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="D117" t="s">
         <v>12</v>
       </c>
       <c r="E117" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="F117" t="s">
         <v>14</v>
       </c>
       <c r="G117" t="s">
-        <v>98</v>
+        <v>15</v>
       </c>
       <c r="H117" t="s">
         <v>12</v>
@@ -3408,22 +3408,22 @@
         <v>12</v>
       </c>
       <c r="B118" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C118" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="D118" t="s">
         <v>12</v>
       </c>
       <c r="E118" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="F118" t="s">
         <v>14</v>
       </c>
       <c r="G118" t="s">
-        <v>44</v>
+        <v>15</v>
       </c>
       <c r="H118" t="s">
         <v>12</v>
@@ -3433,118 +3433,388 @@
       <c r="A119" t="s">
         <v>12</v>
       </c>
+      <c r="B119" t="s">
+        <v>144</v>
+      </c>
+      <c r="C119" t="s">
+        <v>133</v>
+      </c>
+      <c r="D119" t="s">
+        <v>12</v>
+      </c>
+      <c r="E119" t="s">
+        <v>59</v>
+      </c>
+      <c r="F119" t="s">
+        <v>14</v>
+      </c>
+      <c r="G119" t="s">
+        <v>15</v>
+      </c>
+      <c r="H119" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="s">
-        <v>151</v>
+        <v>12</v>
+      </c>
+      <c r="B120" t="s">
+        <v>145</v>
+      </c>
+      <c r="C120" t="s">
+        <v>74</v>
+      </c>
+      <c r="D120" t="s">
+        <v>12</v>
+      </c>
+      <c r="E120" t="s">
+        <v>75</v>
+      </c>
+      <c r="F120" t="s">
+        <v>14</v>
+      </c>
+      <c r="G120" t="s">
+        <v>98</v>
+      </c>
+      <c r="H120" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B121" t="s">
-        <v>2</v>
+        <v>42</v>
       </c>
       <c r="C121" t="s">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="D121" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E121" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="F121" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G121" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="H121" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="s">
-        <v>9</v>
-      </c>
-      <c r="B122" t="s">
-        <v>152</v>
-      </c>
-      <c r="C122" t="s">
-        <v>47</v>
-      </c>
-      <c r="D122" t="s">
-        <v>12</v>
-      </c>
-      <c r="E122" t="s">
-        <v>34</v>
-      </c>
-      <c r="F122" t="s">
-        <v>14</v>
-      </c>
-      <c r="G122" t="s">
-        <v>12</v>
-      </c>
-      <c r="H122" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="s">
-        <v>48</v>
-      </c>
-      <c r="B123" t="s">
-        <v>129</v>
-      </c>
-      <c r="C123" t="s">
-        <v>144</v>
-      </c>
-      <c r="D123" t="s">
-        <v>12</v>
-      </c>
-      <c r="E123" t="s">
-        <v>34</v>
-      </c>
-      <c r="F123" t="s">
-        <v>14</v>
-      </c>
-      <c r="G123" t="s">
-        <v>12</v>
-      </c>
-      <c r="H123" t="s">
-        <v>12</v>
+        <v>146</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="s">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="B124" t="s">
-        <v>153</v>
+        <v>2</v>
       </c>
       <c r="C124" t="s">
-        <v>154</v>
+        <v>3</v>
       </c>
       <c r="D124" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E124" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F124" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="G124" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="H124" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="s">
+        <v>9</v>
+      </c>
+      <c r="B125" t="s">
+        <v>147</v>
+      </c>
+      <c r="C125" t="s">
+        <v>48</v>
+      </c>
+      <c r="D125" t="s">
+        <v>12</v>
+      </c>
+      <c r="E125" t="s">
+        <v>32</v>
+      </c>
+      <c r="F125" t="s">
+        <v>14</v>
+      </c>
+      <c r="G125" t="s">
+        <v>12</v>
+      </c>
+      <c r="H125" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="s">
+        <v>49</v>
+      </c>
+      <c r="B126" t="s">
+        <v>128</v>
+      </c>
+      <c r="C126" t="s">
+        <v>140</v>
+      </c>
+      <c r="D126" t="s">
+        <v>12</v>
+      </c>
+      <c r="E126" t="s">
+        <v>32</v>
+      </c>
+      <c r="F126" t="s">
+        <v>14</v>
+      </c>
+      <c r="G126" t="s">
+        <v>12</v>
+      </c>
+      <c r="H126" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="s">
+        <v>12</v>
+      </c>
+      <c r="B127" t="s">
+        <v>148</v>
+      </c>
+      <c r="C127" t="s">
+        <v>149</v>
+      </c>
+      <c r="D127" t="s">
+        <v>12</v>
+      </c>
+      <c r="E127" t="s">
+        <v>59</v>
+      </c>
+      <c r="F127" t="s">
+        <v>14</v>
+      </c>
+      <c r="G127" t="s">
+        <v>15</v>
+      </c>
+      <c r="H127" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="s">
+        <v>12</v>
+      </c>
+      <c r="B128" t="s">
+        <v>42</v>
+      </c>
+      <c r="C128" t="s">
+        <v>43</v>
+      </c>
+      <c r="D128" t="s">
+        <v>12</v>
+      </c>
+      <c r="E128" t="s">
+        <v>44</v>
+      </c>
+      <c r="F128" t="s">
+        <v>27</v>
+      </c>
+      <c r="G128" t="s">
+        <v>12</v>
+      </c>
+      <c r="H128" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="s">
+        <v>1</v>
+      </c>
+      <c r="B131" t="s">
+        <v>2</v>
+      </c>
+      <c r="C131" t="s">
+        <v>3</v>
+      </c>
+      <c r="D131" t="s">
+        <v>4</v>
+      </c>
+      <c r="E131" t="s">
+        <v>5</v>
+      </c>
+      <c r="F131" t="s">
+        <v>6</v>
+      </c>
+      <c r="G131" t="s">
+        <v>7</v>
+      </c>
+      <c r="H131" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="s">
+        <v>9</v>
+      </c>
+      <c r="B132" t="s">
+        <v>151</v>
+      </c>
+      <c r="C132" t="s">
+        <v>48</v>
+      </c>
+      <c r="D132" t="s">
+        <v>12</v>
+      </c>
+      <c r="E132" t="s">
+        <v>32</v>
+      </c>
+      <c r="F132" t="s">
+        <v>14</v>
+      </c>
+      <c r="G132" t="s">
+        <v>12</v>
+      </c>
+      <c r="H132" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="s">
+        <v>49</v>
+      </c>
+      <c r="B133" t="s">
+        <v>47</v>
+      </c>
+      <c r="C133" t="s">
+        <v>67</v>
+      </c>
+      <c r="D133" t="s">
+        <v>12</v>
+      </c>
+      <c r="E133" t="s">
+        <v>32</v>
+      </c>
+      <c r="F133" t="s">
+        <v>14</v>
+      </c>
+      <c r="G133" t="s">
+        <v>12</v>
+      </c>
+      <c r="H133" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="s">
+        <v>12</v>
+      </c>
+      <c r="B134" t="s">
+        <v>152</v>
+      </c>
+      <c r="C134" t="s">
+        <v>153</v>
+      </c>
+      <c r="D134" t="s">
+        <v>12</v>
+      </c>
+      <c r="E134" t="s">
+        <v>18</v>
+      </c>
+      <c r="F134" t="s">
+        <v>27</v>
+      </c>
+      <c r="G134" t="s">
+        <v>12</v>
+      </c>
+      <c r="H134" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="s">
+        <v>12</v>
+      </c>
+      <c r="B135" t="s">
+        <v>154</v>
+      </c>
+      <c r="C135" t="s">
+        <v>106</v>
+      </c>
+      <c r="D135" t="s">
+        <v>12</v>
+      </c>
+      <c r="E135" t="s">
+        <v>18</v>
+      </c>
+      <c r="F135" t="s">
+        <v>27</v>
+      </c>
+      <c r="G135" t="s">
+        <v>12</v>
+      </c>
+      <c r="H135" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="s">
+        <v>12</v>
+      </c>
+      <c r="B136" t="s">
+        <v>42</v>
+      </c>
+      <c r="C136" t="s">
+        <v>43</v>
+      </c>
+      <c r="D136" t="s">
+        <v>12</v>
+      </c>
+      <c r="E136" t="s">
+        <v>44</v>
+      </c>
+      <c r="F136" t="s">
+        <v>27</v>
+      </c>
+      <c r="G136" t="s">
+        <v>12</v>
+      </c>
+      <c r="H136" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>